<commit_message>
Generate inputs for 2 scenarios to test importance of ET daily timestep.
</commit_message>
<xml_diff>
--- a/SVIHM_Input_Files/Scenario_Development/Scenario Tracking.xlsx
+++ b/SVIHM_Input_Files/Scenario_Development/Scenario Tracking.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20348"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C1C4F84-839E-4CA4-A5F8-C4BDE9A84A5F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{314BA578-960C-4168-89B3-CB4C2443F134}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -435,11 +435,12 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="15.5546875" customWidth="1"/>
     <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5546875" customWidth="1"/>
   </cols>
@@ -483,7 +484,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="2">
-        <v>43692</v>
+        <v>43696</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>6</v>
@@ -497,7 +498,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="2">
-        <v>43692</v>
+        <v>43696</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Scenario cleanup, prepare to run 9 altered precip scenarios
</commit_message>
<xml_diff>
--- a/SVIHM_Input_Files/Scenario_Development/Scenario Tracking.xlsx
+++ b/SVIHM_Input_Files/Scenario_Development/Scenario Tracking.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20348"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{314BA578-960C-4168-89B3-CB4C2443F134}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A8968C9-367E-4519-8636-24778C49772F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
-  <si>
-    <t>Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>up2018</t>
   </si>
@@ -105,6 +102,54 @@
       </rPr>
       <t xml:space="preserve"> spatial CIMIS through April 2015 and then Station 225 Eto. ET record built in SVIHM_input_analyses and original file in SVIHM_Input_Files &gt; Scenario_Development is ref_et_up2018_bmonthly.csv</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Question: Will daily vs monthly ET values make a difference in the water budget? </t>
+  </si>
+  <si>
+    <t>Question/Analysis</t>
+  </si>
+  <si>
+    <t>Scenario Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Result: No visual difference between daily and monthly ET. Overall budgets start to diverge on the 3rd or 4th sigfig. Might as well use the monthly values. </t>
+  </si>
+  <si>
+    <t>Analysis: How different will the 9 ECI273 scenarios make this water budget?</t>
+  </si>
+  <si>
+    <t>pvar_a10</t>
+  </si>
+  <si>
+    <t>pvar_a5</t>
+  </si>
+  <si>
+    <t>pvar_a3</t>
+  </si>
+  <si>
+    <t>pvar_b90</t>
+  </si>
+  <si>
+    <t>pvar_b80</t>
+  </si>
+  <si>
+    <t>pvar_b70</t>
+  </si>
+  <si>
+    <t>pvar_c10</t>
+  </si>
+  <si>
+    <t>pvar_c20</t>
+  </si>
+  <si>
+    <t>pvar_c30</t>
+  </si>
+  <si>
+    <t>hist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Historical precip, gaps filled with ranked regression, created 2019.08.19 (leapdays now included!). Monthly ET (up2018_b). </t>
   </si>
 </sst>
 </file>
@@ -136,7 +181,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -144,14 +189,105 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,79 +568,179 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" customWidth="1"/>
-    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5546875" customWidth="1"/>
+    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.44140625" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <v>43617</v>
+      </c>
+      <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>43617</v>
-      </c>
-      <c r="C2" s="1" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>43692</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
+        <v>43696</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="F4" s="10"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
+        <v>43696</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2">
+      <c r="D5" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="10"/>
+    </row>
+    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="11">
         <v>43696</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="2">
+      <c r="B6" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="13"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
         <v>43696</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="2"/>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Generate 9 precip variation scenarios.
</commit_message>
<xml_diff>
--- a/SVIHM_Input_Files/Scenario_Development/Scenario Tracking.xlsx
+++ b/SVIHM_Input_Files/Scenario_Development/Scenario Tracking.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20348"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A8968C9-367E-4519-8636-24778C49772F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B03BCED-4D87-4A6D-9DFE-1019528490F2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
   <si>
     <t>up2018</t>
   </si>
@@ -122,12 +122,6 @@
     <t>pvar_a10</t>
   </si>
   <si>
-    <t>pvar_a5</t>
-  </si>
-  <si>
-    <t>pvar_a3</t>
-  </si>
-  <si>
     <t>pvar_b90</t>
   </si>
   <si>
@@ -150,6 +144,42 @@
   </si>
   <si>
     <t xml:space="preserve">Historical precip, gaps filled with ranked regression, created 2019.08.19 (leapdays now included!). Monthly ET (up2018_b). </t>
+  </si>
+  <si>
+    <t>pvar_a05</t>
+  </si>
+  <si>
+    <t>pvar_a03</t>
+  </si>
+  <si>
+    <t>Precip and streamflow - dry years 10% drier, water moved onto wet years. Hist ET.</t>
+  </si>
+  <si>
+    <t>Precip and streamflow - dry years 20% drier, water moved onto wet years. Hist ET.</t>
+  </si>
+  <si>
+    <t>Precip and streamflow - dry years 30% drier, water moved onto wet years. Hist ET.</t>
+  </si>
+  <si>
+    <t>Precip - 10 major storms, no other storms. Hist ET and streams.</t>
+  </si>
+  <si>
+    <t>Precip - 5 major storms, no other storms. Hist ET and streams.</t>
+  </si>
+  <si>
+    <t>Precip - 3 major storms, no other storms. Hist ET and streams.</t>
+  </si>
+  <si>
+    <t>Rainy season 90% as large as hist. Hist ET and streams.</t>
+  </si>
+  <si>
+    <t>Rainy season 80% as large as hist. Hist ET and streams.</t>
+  </si>
+  <si>
+    <t>Rainy season 70% as large as hist. Hist ET and streams.</t>
+  </si>
+  <si>
+    <t>SWBM, SVIHM</t>
   </si>
 </sst>
 </file>
@@ -273,7 +303,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -288,6 +318,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -571,7 +602,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -579,7 +610,7 @@
     <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.44140625" customWidth="1"/>
     <col min="3" max="3" width="15.5546875" customWidth="1"/>
-    <col min="4" max="4" width="9.5546875" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -686,13 +717,13 @@
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -700,47 +731,98 @@
         <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>5</v>
+        <v>37</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
-        <v>18</v>
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
-        <v>19</v>
+        <v>27</v>
+      </c>
+      <c r="D11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
-        <v>20</v>
+        <v>18</v>
+      </c>
+      <c r="D12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="D13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
-        <v>22</v>
+        <v>20</v>
+      </c>
+      <c r="D14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
-        <v>23</v>
+        <v>21</v>
+      </c>
+      <c r="D15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="D16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="D17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>